<commit_message>
IF SIMPLE CON ELSE
Todo andando
</commit_message>
<xml_diff>
--- a/Segunda_entrega/CHECK.xlsx
+++ b/Segunda_entrega/CHECK.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="293">
   <si>
     <t>CELDA 1</t>
   </si>
@@ -204,24 +204,6 @@
     <t>Asignacion simple</t>
   </si>
   <si>
-    <t>IF SIMPLE - Condicion</t>
-  </si>
-  <si>
-    <t>IF SIMPLE - Salto por falso</t>
-  </si>
-  <si>
-    <t>IF SIMPLE - Parte True</t>
-  </si>
-  <si>
-    <t>IF con AND - Salto por falso</t>
-  </si>
-  <si>
-    <t>IF con AND - Condicion 1</t>
-  </si>
-  <si>
-    <t>IF con AND - Condicion 2</t>
-  </si>
-  <si>
     <t>CELDA 44</t>
   </si>
   <si>
@@ -231,15 +213,6 @@
     <t>CELDA 51</t>
   </si>
   <si>
-    <t>IF con OR - Condicion 1</t>
-  </si>
-  <si>
-    <t>IF con OR - Condicion 2</t>
-  </si>
-  <si>
-    <t>IF con OR - Salto por falso</t>
-  </si>
-  <si>
     <t>CELDA 42</t>
   </si>
   <si>
@@ -288,10 +261,640 @@
     <t>CELDA 60</t>
   </si>
   <si>
-    <t>IF con OR - Sentencia</t>
-  </si>
-  <si>
-    <t>IF con OR - Salto incondicional al fin del IF</t>
+    <t>CELDA 63</t>
+  </si>
+  <si>
+    <t>CELDA 68</t>
+  </si>
+  <si>
+    <t>CELDA 71</t>
+  </si>
+  <si>
+    <t>CELDA 61</t>
+  </si>
+  <si>
+    <t>CELDA 62</t>
+  </si>
+  <si>
+    <t>CELDA 64</t>
+  </si>
+  <si>
+    <t>CELDA 65</t>
+  </si>
+  <si>
+    <t>CELDA 66</t>
+  </si>
+  <si>
+    <t>CELDA 67</t>
+  </si>
+  <si>
+    <t>CELDA 69</t>
+  </si>
+  <si>
+    <t>CELDA 70</t>
+  </si>
+  <si>
+    <t>CELDA 72</t>
+  </si>
+  <si>
+    <t>CELDA 73</t>
+  </si>
+  <si>
+    <t>CELDA 74</t>
+  </si>
+  <si>
+    <t>CELDA 75</t>
+  </si>
+  <si>
+    <t>CELDA 76</t>
+  </si>
+  <si>
+    <t>CELDA 77</t>
+  </si>
+  <si>
+    <t>CELDA 78</t>
+  </si>
+  <si>
+    <t>CELDA 79</t>
+  </si>
+  <si>
+    <t>CELDA 80</t>
+  </si>
+  <si>
+    <t>CELDA 81</t>
+  </si>
+  <si>
+    <t>CELDA 82</t>
+  </si>
+  <si>
+    <t>CELDA 83</t>
+  </si>
+  <si>
+    <t>CELDA 84</t>
+  </si>
+  <si>
+    <t>CELDA 85</t>
+  </si>
+  <si>
+    <t>CELDA 86</t>
+  </si>
+  <si>
+    <t>CELDA 87</t>
+  </si>
+  <si>
+    <t>CELDA 88</t>
+  </si>
+  <si>
+    <t>CELDA 89</t>
+  </si>
+  <si>
+    <t>CELDA 90</t>
+  </si>
+  <si>
+    <t>CELDA 91</t>
+  </si>
+  <si>
+    <t>CELDA 92</t>
+  </si>
+  <si>
+    <t>CELDA 93</t>
+  </si>
+  <si>
+    <t>CELDA 94</t>
+  </si>
+  <si>
+    <t>CELDA 95</t>
+  </si>
+  <si>
+    <t>CELDA 96</t>
+  </si>
+  <si>
+    <t>CELDA 97</t>
+  </si>
+  <si>
+    <t>CELDA 98</t>
+  </si>
+  <si>
+    <t>CELDA 99</t>
+  </si>
+  <si>
+    <t>CELDA 100</t>
+  </si>
+  <si>
+    <t>CELDA 101</t>
+  </si>
+  <si>
+    <t>CELDA 102</t>
+  </si>
+  <si>
+    <t>CELDA 103</t>
+  </si>
+  <si>
+    <t>CELDA 104</t>
+  </si>
+  <si>
+    <t>CELDA 105</t>
+  </si>
+  <si>
+    <t>CELDA 106</t>
+  </si>
+  <si>
+    <t>CELDA 107</t>
+  </si>
+  <si>
+    <t>CELDA 108</t>
+  </si>
+  <si>
+    <t>CELDA 109</t>
+  </si>
+  <si>
+    <t>CELDA 110</t>
+  </si>
+  <si>
+    <t>CELDA 111</t>
+  </si>
+  <si>
+    <t>CELDA 112</t>
+  </si>
+  <si>
+    <t>CELDA 113</t>
+  </si>
+  <si>
+    <t>CELDA 114</t>
+  </si>
+  <si>
+    <t>CELDA 115</t>
+  </si>
+  <si>
+    <t>CELDA 116</t>
+  </si>
+  <si>
+    <t>CELDA 117</t>
+  </si>
+  <si>
+    <t>CELDA 118</t>
+  </si>
+  <si>
+    <t>CELDA 119</t>
+  </si>
+  <si>
+    <t>CELDA 120</t>
+  </si>
+  <si>
+    <t>CELDA 121</t>
+  </si>
+  <si>
+    <t>CELDA 122</t>
+  </si>
+  <si>
+    <t>CELDA 123</t>
+  </si>
+  <si>
+    <t>CELDA 124</t>
+  </si>
+  <si>
+    <t>CELDA 125</t>
+  </si>
+  <si>
+    <t>CELDA 126</t>
+  </si>
+  <si>
+    <t>CELDA 127</t>
+  </si>
+  <si>
+    <t>CELDA 128</t>
+  </si>
+  <si>
+    <t>CELDA 129</t>
+  </si>
+  <si>
+    <t>CELDA 130</t>
+  </si>
+  <si>
+    <t>CELDA 131</t>
+  </si>
+  <si>
+    <t>CELDA 132</t>
+  </si>
+  <si>
+    <t>CELDA 133</t>
+  </si>
+  <si>
+    <t>CELDA 134</t>
+  </si>
+  <si>
+    <t>CELDA 135</t>
+  </si>
+  <si>
+    <t>CELDA 136</t>
+  </si>
+  <si>
+    <t>CELDA 137</t>
+  </si>
+  <si>
+    <t>CELDA 138</t>
+  </si>
+  <si>
+    <t>CELDA 139</t>
+  </si>
+  <si>
+    <t>CELDA 140</t>
+  </si>
+  <si>
+    <t>CELDA 141</t>
+  </si>
+  <si>
+    <t>CELDA 142</t>
+  </si>
+  <si>
+    <t>CELDA 143</t>
+  </si>
+  <si>
+    <t>CELDA 144</t>
+  </si>
+  <si>
+    <t>CELDA 145</t>
+  </si>
+  <si>
+    <t>CELDA 146</t>
+  </si>
+  <si>
+    <t>CELDA 147</t>
+  </si>
+  <si>
+    <t>CELDA 148</t>
+  </si>
+  <si>
+    <t>CELDA 149</t>
+  </si>
+  <si>
+    <t>CELDA 150</t>
+  </si>
+  <si>
+    <t>CELDA 151</t>
+  </si>
+  <si>
+    <t>CELDA 152</t>
+  </si>
+  <si>
+    <t>CELDA 153</t>
+  </si>
+  <si>
+    <t>CELDA 154</t>
+  </si>
+  <si>
+    <t>CELDA 155</t>
+  </si>
+  <si>
+    <t>CELDA 156</t>
+  </si>
+  <si>
+    <t>CELDA 157</t>
+  </si>
+  <si>
+    <t>CELDA 158</t>
+  </si>
+  <si>
+    <t>CELDA 159</t>
+  </si>
+  <si>
+    <t>CELDA 160</t>
+  </si>
+  <si>
+    <t>CELDA 161</t>
+  </si>
+  <si>
+    <t>CELDA 162</t>
+  </si>
+  <si>
+    <t>CELDA 163</t>
+  </si>
+  <si>
+    <t>CELDA 164</t>
+  </si>
+  <si>
+    <t>CELDA 165</t>
+  </si>
+  <si>
+    <t>CELDA 166</t>
+  </si>
+  <si>
+    <t>CELDA 167</t>
+  </si>
+  <si>
+    <t>CELDA 168</t>
+  </si>
+  <si>
+    <t>CELDA 169</t>
+  </si>
+  <si>
+    <t>CELDA 170</t>
+  </si>
+  <si>
+    <t>CELDA 171</t>
+  </si>
+  <si>
+    <t>CELDA 172</t>
+  </si>
+  <si>
+    <t>CELDA 173</t>
+  </si>
+  <si>
+    <t>CELDA 174</t>
+  </si>
+  <si>
+    <t>CELDA 175</t>
+  </si>
+  <si>
+    <t>CELDA 176</t>
+  </si>
+  <si>
+    <t>CELDA 177</t>
+  </si>
+  <si>
+    <t>CELDA 178</t>
+  </si>
+  <si>
+    <t>CELDA 179</t>
+  </si>
+  <si>
+    <t>CELDA 180</t>
+  </si>
+  <si>
+    <t>CELDA 181</t>
+  </si>
+  <si>
+    <t>CELDA 182</t>
+  </si>
+  <si>
+    <t>CELDA 183</t>
+  </si>
+  <si>
+    <t>CELDA 184</t>
+  </si>
+  <si>
+    <t>CELDA 185</t>
+  </si>
+  <si>
+    <t>CELDA 186</t>
+  </si>
+  <si>
+    <t>CELDA 187</t>
+  </si>
+  <si>
+    <t>CELDA 188</t>
+  </si>
+  <si>
+    <t>CELDA 189</t>
+  </si>
+  <si>
+    <t>CELDA 190</t>
+  </si>
+  <si>
+    <t>CELDA 191</t>
+  </si>
+  <si>
+    <t>CELDA 192</t>
+  </si>
+  <si>
+    <t>CELDA 193</t>
+  </si>
+  <si>
+    <t>CELDA 194</t>
+  </si>
+  <si>
+    <t>CELDA 195</t>
+  </si>
+  <si>
+    <t>CELDA 196</t>
+  </si>
+  <si>
+    <t>CELDA 197</t>
+  </si>
+  <si>
+    <t>CELDA 198</t>
+  </si>
+  <si>
+    <t>CELDA 199</t>
+  </si>
+  <si>
+    <t>CELDA 200</t>
+  </si>
+  <si>
+    <t>CELDA 201</t>
+  </si>
+  <si>
+    <t>CELDA 202</t>
+  </si>
+  <si>
+    <t>CELDA 203</t>
+  </si>
+  <si>
+    <t>CELDA 204</t>
+  </si>
+  <si>
+    <t>CELDA 205</t>
+  </si>
+  <si>
+    <t>CELDA 206</t>
+  </si>
+  <si>
+    <t>CELDA 207</t>
+  </si>
+  <si>
+    <t>CELDA 208</t>
+  </si>
+  <si>
+    <t>CELDA 209</t>
+  </si>
+  <si>
+    <t>CELDA 210</t>
+  </si>
+  <si>
+    <t>CELDA 211</t>
+  </si>
+  <si>
+    <t>CELDA 212</t>
+  </si>
+  <si>
+    <t>CELDA 213</t>
+  </si>
+  <si>
+    <t>CELDA 214</t>
+  </si>
+  <si>
+    <t>CELDA 215</t>
+  </si>
+  <si>
+    <t>CELDA 216</t>
+  </si>
+  <si>
+    <t>CELDA 217</t>
+  </si>
+  <si>
+    <t>CELDA 218</t>
+  </si>
+  <si>
+    <t>CELDA 219</t>
+  </si>
+  <si>
+    <t>CELDA 220</t>
+  </si>
+  <si>
+    <t>CELDA 221</t>
+  </si>
+  <si>
+    <t>CELDA 222</t>
+  </si>
+  <si>
+    <t>CELDA 223</t>
+  </si>
+  <si>
+    <t>CELDA 224</t>
+  </si>
+  <si>
+    <t>CELDA 225</t>
+  </si>
+  <si>
+    <t>CELDA 226</t>
+  </si>
+  <si>
+    <t>CELDA 227</t>
+  </si>
+  <si>
+    <t>CELDA 228</t>
+  </si>
+  <si>
+    <t>CELDA 229</t>
+  </si>
+  <si>
+    <t>CELDA 230</t>
+  </si>
+  <si>
+    <t>CELDA 231</t>
+  </si>
+  <si>
+    <t>CELDA 232</t>
+  </si>
+  <si>
+    <t>CELDA 233</t>
+  </si>
+  <si>
+    <t>CELDA 234</t>
+  </si>
+  <si>
+    <t>CELDA 235</t>
+  </si>
+  <si>
+    <t>CELDA 236</t>
+  </si>
+  <si>
+    <t>CELDA 237</t>
+  </si>
+  <si>
+    <t>CELDA 238</t>
+  </si>
+  <si>
+    <t>CELDA 239</t>
+  </si>
+  <si>
+    <t>CELDA 240</t>
+  </si>
+  <si>
+    <t>CELDA 241</t>
+  </si>
+  <si>
+    <t>CELDA 242</t>
+  </si>
+  <si>
+    <t>CELDA 243</t>
+  </si>
+  <si>
+    <t>CELDA 244</t>
+  </si>
+  <si>
+    <t>CELDA 245</t>
+  </si>
+  <si>
+    <t>CELDA 246</t>
+  </si>
+  <si>
+    <t>CELDA 247</t>
+  </si>
+  <si>
+    <t>CELDA 248</t>
+  </si>
+  <si>
+    <t>CELDA 249</t>
+  </si>
+  <si>
+    <t>CELDA 250</t>
+  </si>
+  <si>
+    <t>CELDA 251</t>
+  </si>
+  <si>
+    <t>CELDA 252</t>
+  </si>
+  <si>
+    <t>CELDA 253</t>
+  </si>
+  <si>
+    <t>CELDA 254</t>
+  </si>
+  <si>
+    <t>CELDA 255</t>
+  </si>
+  <si>
+    <t>CELDA 256</t>
+  </si>
+  <si>
+    <t>CELDA 257</t>
+  </si>
+  <si>
+    <t>CELDA 258</t>
+  </si>
+  <si>
+    <t>CELDA 259</t>
+  </si>
+  <si>
+    <t>CELDA 260</t>
+  </si>
+  <si>
+    <t>CELDA 261</t>
+  </si>
+  <si>
+    <t>CELDA 262</t>
+  </si>
+  <si>
+    <t>CELDA 263</t>
+  </si>
+  <si>
+    <t>CELDA 264</t>
+  </si>
+  <si>
+    <t>CELDA 265</t>
+  </si>
+  <si>
+    <t>CELDA 266</t>
+  </si>
+  <si>
+    <t>IF SIMPLE</t>
+  </si>
+  <si>
+    <t>IF DOBLE CON or</t>
+  </si>
+  <si>
+    <t>IF DOBLE CON OR</t>
+  </si>
+  <si>
+    <t>IF DOBLE CON and</t>
+  </si>
+  <si>
+    <t>IF DOBLE CON AND</t>
+  </si>
+  <si>
+    <t>IF SIMPLE CON ELSE</t>
   </si>
 </sst>
 </file>
@@ -315,7 +918,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +946,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,15 +1030,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -439,10 +1043,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -454,11 +1058,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1088,7 +1697,7 @@
       <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="2" t="str">
@@ -1106,7 +1715,7 @@
       <c r="C21" s="1">
         <v>7</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1122,7 +1731,7 @@
       <c r="C22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1138,7 +1747,7 @@
       <c r="C23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1172,7 +1781,7 @@
       <c r="C25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>48</v>
       </c>
       <c r="E25" s="2" t="str">
@@ -1190,7 +1799,7 @@
       <c r="C26" s="1">
         <v>8</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1206,7 +1815,7 @@
       <c r="C27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1222,7 +1831,7 @@
       <c r="C28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1256,7 +1865,7 @@
       <c r="C30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="11" t="s">
         <v>50</v>
       </c>
       <c r="E30" s="2" t="str">
@@ -1274,7 +1883,7 @@
       <c r="C31" s="1">
         <v>5</v>
       </c>
-      <c r="D31" s="12"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1290,7 +1899,7 @@
       <c r="C32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="12"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1306,7 +1915,7 @@
       <c r="C33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1322,7 +1931,7 @@
       <c r="C34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="12"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1338,7 +1947,7 @@
       <c r="C35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E35" s="2" t="str">
@@ -1356,7 +1965,7 @@
       <c r="C36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="11"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1381,16 +1990,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:F267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72:D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="11.42578125" style="18"/>
+    <col min="3" max="3" width="11.42578125" style="17"/>
     <col min="4" max="4" width="29" style="6" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="2"/>
   </cols>
@@ -1416,14 +2025,14 @@
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="2" t="str">
-        <f t="shared" ref="E2:E61" si="0">IF(B2=C2,"OK","ERROR")</f>
+        <f t="shared" ref="E2:E65" si="0">IF(B2=C2,"OK","ERROR")</f>
         <v>OK</v>
       </c>
     </row>
@@ -1434,10 +2043,10 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>1</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1450,10 +2059,10 @@
       <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="15"/>
       <c r="E4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1466,10 +2075,10 @@
       <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>61</v>
       </c>
       <c r="E5" s="2" t="str">
@@ -1484,10 +2093,10 @@
       <c r="B6" s="1">
         <v>10</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>10</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1500,10 +2109,10 @@
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1516,11 +2125,11 @@
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>62</v>
+      <c r="D8" s="16" t="s">
+        <v>287</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1534,10 +2143,10 @@
       <c r="B9" s="1">
         <v>15</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>15</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1550,10 +2159,10 @@
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1566,10 +2175,10 @@
       <c r="B11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="17"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1582,12 +2191,10 @@
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="D12" s="16"/>
       <c r="E12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1600,12 +2207,10 @@
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>64</v>
-      </c>
+      <c r="D13" s="16"/>
       <c r="E13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1618,10 +2223,10 @@
       <c r="B14" s="1">
         <v>16</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>16</v>
       </c>
-      <c r="D14" s="17"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1634,10 +2239,10 @@
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1650,11 +2255,11 @@
       <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>66</v>
+        <v>291</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1668,7 +2273,7 @@
       <c r="B17" s="1">
         <v>15</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="17">
         <v>15</v>
       </c>
       <c r="D17" s="13"/>
@@ -1684,7 +2289,7 @@
       <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="13"/>
@@ -1700,7 +2305,7 @@
       <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="13"/>
@@ -1716,12 +2321,10 @@
       <c r="B20" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>65</v>
-      </c>
+      <c r="D20" s="13"/>
       <c r="E20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1734,12 +2337,10 @@
       <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>67</v>
-      </c>
+      <c r="D21" s="13"/>
       <c r="E21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1752,7 +2353,7 @@
       <c r="B22" s="1">
         <v>4</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="17">
         <v>4</v>
       </c>
       <c r="D22" s="13"/>
@@ -1768,7 +2369,7 @@
       <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="13"/>
@@ -1784,7 +2385,7 @@
       <c r="B24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="13"/>
@@ -1800,12 +2401,10 @@
       <c r="B25" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>65</v>
-      </c>
+      <c r="D25" s="13"/>
       <c r="E25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1818,12 +2417,10 @@
       <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>64</v>
-      </c>
+      <c r="D26" s="13"/>
       <c r="E26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1836,7 +2433,7 @@
       <c r="B27" s="1">
         <v>16</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="17">
         <v>16</v>
       </c>
       <c r="D27" s="13"/>
@@ -1852,7 +2449,7 @@
       <c r="B28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>34</v>
       </c>
       <c r="D28" s="13"/>
@@ -1868,11 +2465,11 @@
       <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>66</v>
+      <c r="D29" s="12" t="s">
+        <v>290</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1886,10 +2483,10 @@
       <c r="B30" s="1">
         <v>15</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="17">
         <v>15</v>
       </c>
-      <c r="D30" s="14"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1902,10 +2499,10 @@
       <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="14"/>
+      <c r="D31" s="12"/>
       <c r="E31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -1918,337 +2515,320 @@
       <c r="B32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="14"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="D33" s="12"/>
       <c r="E33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="D34" s="12"/>
       <c r="E34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
       <c r="B35" s="1">
         <v>4</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="17">
         <v>4</v>
       </c>
-      <c r="D35" s="14"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="14"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="14"/>
+      <c r="D37" s="12"/>
       <c r="E37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="D38" s="12"/>
       <c r="E38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="D39" s="12"/>
       <c r="E39" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>59</v>
       </c>
       <c r="B40" s="1">
         <v>16</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="17">
         <v>16</v>
       </c>
-      <c r="D40" s="14"/>
+      <c r="D40" s="12"/>
       <c r="E40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="14"/>
+      <c r="D41" s="12"/>
       <c r="E41" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="14" t="s">
-        <v>71</v>
+      <c r="D42" s="19" t="s">
+        <v>289</v>
       </c>
       <c r="E42" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B43" s="1">
         <v>15</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C43" s="17">
         <v>15</v>
       </c>
-      <c r="D43" s="14"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="14"/>
+      <c r="D44" s="19"/>
       <c r="E44" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="G44">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="14"/>
+      <c r="D45" s="19"/>
       <c r="E45" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>73</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="19"/>
       <c r="E46" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="14" t="s">
-        <v>90</v>
-      </c>
+      <c r="D47" s="19"/>
       <c r="E47" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="F47" s="19"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D48" s="14"/>
+        <v>73</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="19"/>
       <c r="E48" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="F48" s="19"/>
+      <c r="F48" s="8"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C49" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D49" s="14"/>
+      <c r="D49" s="19"/>
       <c r="E49" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="F49" s="19"/>
+      <c r="F49" s="8"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B50" s="1">
         <v>4</v>
       </c>
-      <c r="C50" s="18">
+      <c r="C50" s="17">
         <v>4</v>
       </c>
-      <c r="D50" s="14"/>
+      <c r="D50" s="19"/>
       <c r="E50" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
-      <c r="F50" s="19"/>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C51" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D51" s="20" t="s">
-        <v>91</v>
-      </c>
+      <c r="D51" s="19"/>
       <c r="E51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2256,17 +2836,15 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D52" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="D52" s="19"/>
       <c r="E52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2274,15 +2852,15 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D53" s="14"/>
+        <v>76</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="19"/>
       <c r="E53" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2290,15 +2868,15 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="18" t="s">
+      <c r="C54" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="14"/>
+      <c r="D54" s="19"/>
       <c r="E54" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2306,15 +2884,15 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B55" s="1">
         <v>16</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C55" s="17">
         <v>16</v>
       </c>
-      <c r="D55" s="14"/>
+      <c r="D55" s="19"/>
       <c r="E55" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2322,41 +2900,49 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="C56" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="D56" s="19"/>
       <c r="E56" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>76</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>33</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>91</v>
+        <v>288</v>
       </c>
       <c r="E57" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>86</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>91</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B58" s="18">
+        <v>15</v>
+      </c>
+      <c r="C58" s="17">
+        <v>15</v>
+      </c>
+      <c r="D58" s="20"/>
       <c r="E58" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2364,8 +2950,15 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="20"/>
       <c r="E59" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2373,8 +2966,15 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>88</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="20"/>
       <c r="E60" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2382,28 +2982,2047 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="20"/>
+      <c r="E61" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="20"/>
+      <c r="E63" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D64" s="20"/>
+      <c r="E64" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" s="18">
+        <v>4</v>
+      </c>
+      <c r="C65" s="17">
+        <v>4</v>
+      </c>
+      <c r="D65" s="20"/>
+      <c r="E65" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" s="20"/>
+      <c r="E66" s="2" t="str">
+        <f t="shared" ref="E66:E129" si="1">IF(B66=C66,"OK","ERROR")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>89</v>
       </c>
-      <c r="E61" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="B68" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D68" s="20"/>
+      <c r="E68" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" s="20"/>
+      <c r="E69" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>90</v>
+      </c>
+      <c r="B70" s="1">
+        <v>16</v>
+      </c>
+      <c r="C70" s="17">
+        <v>16</v>
+      </c>
+      <c r="D70" s="20"/>
+      <c r="E70" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="20"/>
+      <c r="E71" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E72" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" s="1">
+        <v>15</v>
+      </c>
+      <c r="C73" s="17">
+        <v>15</v>
+      </c>
+      <c r="D73" s="13"/>
+      <c r="E73" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>93</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D74" s="13"/>
+      <c r="E74" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D75" s="13"/>
+      <c r="E75" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>95</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D76" s="13"/>
+      <c r="E76" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>96</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="13"/>
+      <c r="E77" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" s="1">
+        <v>16</v>
+      </c>
+      <c r="C78" s="17">
+        <v>16</v>
+      </c>
+      <c r="D78" s="13"/>
+      <c r="E78" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>98</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D79" s="13"/>
+      <c r="E79" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>99</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D80" s="13"/>
+      <c r="E80" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D81" s="13"/>
+      <c r="E81" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>101</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" s="13"/>
+      <c r="E82" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83" s="1">
+        <v>17</v>
+      </c>
+      <c r="C83" s="17">
+        <v>17</v>
+      </c>
+      <c r="D83" s="13"/>
+      <c r="E83" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D84" s="13"/>
+      <c r="E84" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>104</v>
+      </c>
+      <c r="E85" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>105</v>
+      </c>
+      <c r="E86" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>106</v>
+      </c>
+      <c r="E87" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>107</v>
+      </c>
+      <c r="E88" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>108</v>
+      </c>
+      <c r="E89" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>109</v>
+      </c>
+      <c r="E90" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>110</v>
+      </c>
+      <c r="E91" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>111</v>
+      </c>
+      <c r="E92" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>112</v>
+      </c>
+      <c r="E93" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>113</v>
+      </c>
+      <c r="E94" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>114</v>
+      </c>
+      <c r="E95" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>115</v>
+      </c>
+      <c r="E96" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>116</v>
+      </c>
+      <c r="E97" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>117</v>
+      </c>
+      <c r="E98" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>118</v>
+      </c>
+      <c r="E99" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>119</v>
+      </c>
+      <c r="E100" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>120</v>
+      </c>
+      <c r="E101" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>121</v>
+      </c>
+      <c r="E102" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>122</v>
+      </c>
+      <c r="E103" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>123</v>
+      </c>
+      <c r="E104" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>124</v>
+      </c>
+      <c r="E105" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>125</v>
+      </c>
+      <c r="E106" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>126</v>
+      </c>
+      <c r="E107" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>127</v>
+      </c>
+      <c r="E108" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>128</v>
+      </c>
+      <c r="E109" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>129</v>
+      </c>
+      <c r="E110" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>130</v>
+      </c>
+      <c r="E111" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>131</v>
+      </c>
+      <c r="E112" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>132</v>
+      </c>
+      <c r="E113" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>133</v>
+      </c>
+      <c r="E114" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>134</v>
+      </c>
+      <c r="E115" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>135</v>
+      </c>
+      <c r="E116" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>136</v>
+      </c>
+      <c r="E117" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>137</v>
+      </c>
+      <c r="E118" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>138</v>
+      </c>
+      <c r="E119" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>139</v>
+      </c>
+      <c r="E120" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>140</v>
+      </c>
+      <c r="E121" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>141</v>
+      </c>
+      <c r="E122" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>142</v>
+      </c>
+      <c r="E123" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>143</v>
+      </c>
+      <c r="E124" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>144</v>
+      </c>
+      <c r="E125" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>145</v>
+      </c>
+      <c r="E126" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>146</v>
+      </c>
+      <c r="E127" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>147</v>
+      </c>
+      <c r="E128" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>148</v>
+      </c>
+      <c r="E129" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>149</v>
+      </c>
+      <c r="E130" s="2" t="str">
+        <f t="shared" ref="E130:E193" si="2">IF(B130=C130,"OK","ERROR")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>150</v>
+      </c>
+      <c r="E131" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>151</v>
+      </c>
+      <c r="E132" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>152</v>
+      </c>
+      <c r="E133" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>153</v>
+      </c>
+      <c r="E134" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>154</v>
+      </c>
+      <c r="E135" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>155</v>
+      </c>
+      <c r="E136" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>156</v>
+      </c>
+      <c r="E137" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>157</v>
+      </c>
+      <c r="E138" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>158</v>
+      </c>
+      <c r="E139" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>159</v>
+      </c>
+      <c r="E140" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>160</v>
+      </c>
+      <c r="E141" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>161</v>
+      </c>
+      <c r="E142" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>162</v>
+      </c>
+      <c r="E143" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>163</v>
+      </c>
+      <c r="E144" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>164</v>
+      </c>
+      <c r="E145" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>165</v>
+      </c>
+      <c r="E146" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>166</v>
+      </c>
+      <c r="E147" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>167</v>
+      </c>
+      <c r="E148" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>168</v>
+      </c>
+      <c r="E149" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>169</v>
+      </c>
+      <c r="E150" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>170</v>
+      </c>
+      <c r="E151" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>171</v>
+      </c>
+      <c r="E152" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>172</v>
+      </c>
+      <c r="E153" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>173</v>
+      </c>
+      <c r="E154" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>174</v>
+      </c>
+      <c r="E155" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>175</v>
+      </c>
+      <c r="E156" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>176</v>
+      </c>
+      <c r="E157" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>177</v>
+      </c>
+      <c r="E158" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>178</v>
+      </c>
+      <c r="E159" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>179</v>
+      </c>
+      <c r="E160" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>180</v>
+      </c>
+      <c r="E161" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>181</v>
+      </c>
+      <c r="E162" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>182</v>
+      </c>
+      <c r="E163" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>183</v>
+      </c>
+      <c r="E164" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>184</v>
+      </c>
+      <c r="E165" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>185</v>
+      </c>
+      <c r="E166" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>186</v>
+      </c>
+      <c r="E167" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>187</v>
+      </c>
+      <c r="E168" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>188</v>
+      </c>
+      <c r="E169" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>189</v>
+      </c>
+      <c r="E170" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>190</v>
+      </c>
+      <c r="E171" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>191</v>
+      </c>
+      <c r="E172" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>192</v>
+      </c>
+      <c r="E173" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>193</v>
+      </c>
+      <c r="E174" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>194</v>
+      </c>
+      <c r="E175" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>195</v>
+      </c>
+      <c r="E176" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>196</v>
+      </c>
+      <c r="E177" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>197</v>
+      </c>
+      <c r="E178" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>198</v>
+      </c>
+      <c r="E179" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>199</v>
+      </c>
+      <c r="E180" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>200</v>
+      </c>
+      <c r="E181" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>201</v>
+      </c>
+      <c r="E182" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>202</v>
+      </c>
+      <c r="E183" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>203</v>
+      </c>
+      <c r="E184" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>204</v>
+      </c>
+      <c r="E185" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>205</v>
+      </c>
+      <c r="E186" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>206</v>
+      </c>
+      <c r="E187" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>207</v>
+      </c>
+      <c r="E188" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>208</v>
+      </c>
+      <c r="E189" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>209</v>
+      </c>
+      <c r="E190" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>210</v>
+      </c>
+      <c r="E191" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>211</v>
+      </c>
+      <c r="E192" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>212</v>
+      </c>
+      <c r="E193" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>213</v>
+      </c>
+      <c r="E194" s="2" t="str">
+        <f t="shared" ref="E194:E257" si="3">IF(B194=C194,"OK","ERROR")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>214</v>
+      </c>
+      <c r="E195" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>215</v>
+      </c>
+      <c r="E196" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>216</v>
+      </c>
+      <c r="E197" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>217</v>
+      </c>
+      <c r="E198" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>218</v>
+      </c>
+      <c r="E199" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>219</v>
+      </c>
+      <c r="E200" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>220</v>
+      </c>
+      <c r="E201" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>221</v>
+      </c>
+      <c r="E202" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>222</v>
+      </c>
+      <c r="E203" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>223</v>
+      </c>
+      <c r="E204" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>224</v>
+      </c>
+      <c r="E205" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>225</v>
+      </c>
+      <c r="E206" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>226</v>
+      </c>
+      <c r="E207" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>227</v>
+      </c>
+      <c r="E208" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>228</v>
+      </c>
+      <c r="E209" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>229</v>
+      </c>
+      <c r="E210" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>230</v>
+      </c>
+      <c r="E211" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>231</v>
+      </c>
+      <c r="E212" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>232</v>
+      </c>
+      <c r="E213" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>233</v>
+      </c>
+      <c r="E214" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>234</v>
+      </c>
+      <c r="E215" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>235</v>
+      </c>
+      <c r="E216" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>236</v>
+      </c>
+      <c r="E217" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>237</v>
+      </c>
+      <c r="E218" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>238</v>
+      </c>
+      <c r="E219" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>239</v>
+      </c>
+      <c r="E220" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>240</v>
+      </c>
+      <c r="E221" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>241</v>
+      </c>
+      <c r="E222" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>242</v>
+      </c>
+      <c r="E223" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>243</v>
+      </c>
+      <c r="E224" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>244</v>
+      </c>
+      <c r="E225" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>245</v>
+      </c>
+      <c r="E226" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>246</v>
+      </c>
+      <c r="E227" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>247</v>
+      </c>
+      <c r="E228" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>248</v>
+      </c>
+      <c r="E229" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>249</v>
+      </c>
+      <c r="E230" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>250</v>
+      </c>
+      <c r="E231" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>251</v>
+      </c>
+      <c r="E232" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>252</v>
+      </c>
+      <c r="E233" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>253</v>
+      </c>
+      <c r="E234" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>254</v>
+      </c>
+      <c r="E235" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>255</v>
+      </c>
+      <c r="E236" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>256</v>
+      </c>
+      <c r="E237" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>257</v>
+      </c>
+      <c r="E238" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>258</v>
+      </c>
+      <c r="E239" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>259</v>
+      </c>
+      <c r="E240" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>260</v>
+      </c>
+      <c r="E241" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>261</v>
+      </c>
+      <c r="E242" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>262</v>
+      </c>
+      <c r="E243" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>263</v>
+      </c>
+      <c r="E244" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>264</v>
+      </c>
+      <c r="E245" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>265</v>
+      </c>
+      <c r="E246" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>266</v>
+      </c>
+      <c r="E247" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>267</v>
+      </c>
+      <c r="E248" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>268</v>
+      </c>
+      <c r="E249" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>269</v>
+      </c>
+      <c r="E250" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>270</v>
+      </c>
+      <c r="E251" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>271</v>
+      </c>
+      <c r="E252" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>272</v>
+      </c>
+      <c r="E253" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>273</v>
+      </c>
+      <c r="E254" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>274</v>
+      </c>
+      <c r="E255" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>275</v>
+      </c>
+      <c r="E256" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>276</v>
+      </c>
+      <c r="E257" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>277</v>
+      </c>
+      <c r="E258" s="2" t="str">
+        <f t="shared" ref="E258:E267" si="4">IF(B258=C258,"OK","ERROR")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>278</v>
+      </c>
+      <c r="E259" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>279</v>
+      </c>
+      <c r="E260" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>280</v>
+      </c>
+      <c r="E261" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>281</v>
+      </c>
+      <c r="E262" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>282</v>
+      </c>
+      <c r="E263" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>283</v>
+      </c>
+      <c r="E264" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>284</v>
+      </c>
+      <c r="E265" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>285</v>
+      </c>
+      <c r="E266" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>286</v>
+      </c>
+      <c r="E267" s="2" t="str">
+        <f t="shared" si="4"/>
         <v>OK</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="D39:D41"/>
+  <mergeCells count="8">
+    <mergeCell ref="D57:D71"/>
+    <mergeCell ref="D72:D84"/>
+    <mergeCell ref="D29:D41"/>
+    <mergeCell ref="D16:D28"/>
+    <mergeCell ref="D8:D15"/>
+    <mergeCell ref="D42:D56"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D21:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ASIGNACION MULTIPLE en GCI
Solo faltaria actualizar la tabla de simbolos
</commit_message>
<xml_diff>
--- a/Segunda_entrega/CHECK.xlsx
+++ b/Segunda_entrega/CHECK.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mauro\Cloud\GitHub\Compilador\Segunda_Entrega\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="45" windowWidth="11715" windowHeight="4950"/>
   </bookViews>
@@ -10,8 +15,9 @@
     <sheet name="TEST COMPLETO" sheetId="2" r:id="rId1"/>
     <sheet name="TEST-IF" sheetId="3" r:id="rId2"/>
     <sheet name="TEST-WHILE" sheetId="4" r:id="rId3"/>
+    <sheet name="TEST-ASIGMUL" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -21,7 +27,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="F2" authorId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0">
+    <comment ref="M2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -148,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0">
+    <comment ref="M5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0">
+    <comment ref="N5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0">
+    <comment ref="Q5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -273,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0">
+    <comment ref="F8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0">
+    <comment ref="H8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -321,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0">
+    <comment ref="I8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -345,7 +351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M8" authorId="0">
+    <comment ref="M8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -369,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0">
+    <comment ref="O8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -393,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0">
+    <comment ref="P8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -417,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T8" authorId="0">
+    <comment ref="T8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -441,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U8" authorId="0">
+    <comment ref="U8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -465,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -489,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0">
+    <comment ref="H11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -513,7 +519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0">
+    <comment ref="I11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -537,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="0">
+    <comment ref="M11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -561,7 +567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O11" authorId="0">
+    <comment ref="O11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -585,7 +591,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P11" authorId="0">
+    <comment ref="P11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -609,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T11" authorId="0">
+    <comment ref="T11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -633,7 +639,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U11" authorId="0">
+    <comment ref="U11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -662,7 +668,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="307">
   <si>
     <t>CELDA 1</t>
   </si>
@@ -1565,12 +1571,31 @@
   </si>
   <si>
     <t>1° desapilado -&gt; parte verdadera</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>###</t>
+  </si>
+  <si>
+    <t>i:=1 
+b:=10</t>
+  </si>
+  <si>
+    <t>desapilo y asigno</t>
+  </si>
+  <si>
+    <t>a:=b:=i:=8</t>
+  </si>
+  <si>
+    <t>ASIGNACION MULTIPLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1623,7 +1648,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1692,18 +1717,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1796,11 +1827,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1872,7 +1936,16 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1881,7 +1954,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1894,9 +1973,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1927,6 +2003,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1963,6 +2054,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2011,7 +2105,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2046,7 +2140,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2258,7 +2352,7 @@
   <dimension ref="A1:H267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D8" sqref="D8:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,7 +2390,7 @@
       <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="29" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="6" t="str">
@@ -2321,7 +2415,7 @@
       <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="6" t="str">
         <f t="shared" ref="E3:E66" si="0">IF(AND(B3=C3,B3&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -2337,7 +2431,7 @@
       <c r="C4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="35"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2353,7 +2447,7 @@
       <c r="C5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="29" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="6" t="str">
@@ -2371,7 +2465,7 @@
       <c r="C6" s="7">
         <v>10</v>
       </c>
-      <c r="D6" s="35"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2387,7 +2481,7 @@
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2403,7 +2497,7 @@
       <c r="C8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="36" t="s">
         <v>281</v>
       </c>
       <c r="E8" s="6" t="str">
@@ -2421,7 +2515,7 @@
       <c r="C9" s="7">
         <v>15</v>
       </c>
-      <c r="D9" s="31"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2437,7 +2531,7 @@
       <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="31"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2453,7 +2547,7 @@
       <c r="C11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2469,7 +2563,7 @@
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2485,7 +2579,7 @@
       <c r="C13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="31"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2501,7 +2595,7 @@
       <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="31"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2517,7 +2611,7 @@
       <c r="C15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="31"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2533,7 +2627,7 @@
       <c r="C16" s="7">
         <v>16</v>
       </c>
-      <c r="D16" s="31"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2549,7 +2643,7 @@
       <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="31"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2565,7 +2659,7 @@
       <c r="C18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2581,7 +2675,7 @@
       <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="31"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2597,7 +2691,7 @@
       <c r="C20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="31" t="s">
         <v>282</v>
       </c>
       <c r="E20" s="6" t="str">
@@ -2615,7 +2709,7 @@
       <c r="C21" s="7">
         <v>15</v>
       </c>
-      <c r="D21" s="29"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2631,7 +2725,7 @@
       <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="32"/>
       <c r="E22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2647,7 +2741,7 @@
       <c r="C23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="29"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2663,7 +2757,7 @@
       <c r="C24" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="29"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2679,7 +2773,7 @@
       <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="29"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2695,7 +2789,7 @@
       <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="29"/>
+      <c r="D26" s="32"/>
       <c r="E26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2711,7 +2805,7 @@
       <c r="C27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="32"/>
       <c r="E27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2727,7 +2821,7 @@
       <c r="C28" s="7">
         <v>16</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="32"/>
       <c r="E28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2743,7 +2837,7 @@
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2759,7 +2853,7 @@
       <c r="C30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2775,7 +2869,7 @@
       <c r="C31" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="29"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2791,7 +2885,7 @@
       <c r="C32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="29"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2807,7 +2901,7 @@
       <c r="C33" s="7">
         <v>17</v>
       </c>
-      <c r="D33" s="29"/>
+      <c r="D33" s="32"/>
       <c r="E33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2823,7 +2917,7 @@
       <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="29"/>
+      <c r="D34" s="32"/>
       <c r="E34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2839,7 +2933,7 @@
       <c r="C35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="36" t="s">
         <v>291</v>
       </c>
       <c r="E35" s="6" t="str">
@@ -2857,7 +2951,7 @@
       <c r="C36" s="7">
         <v>15</v>
       </c>
-      <c r="D36" s="32"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2873,7 +2967,7 @@
       <c r="C37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="32"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2889,7 +2983,7 @@
       <c r="C38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="32"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2905,7 +2999,7 @@
       <c r="C39" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="32"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2921,7 +3015,7 @@
       <c r="C40" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="32"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2937,7 +3031,7 @@
       <c r="C41" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D41" s="32"/>
+      <c r="D41" s="37"/>
       <c r="E41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2953,7 +3047,7 @@
       <c r="C42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="32"/>
+      <c r="D42" s="37"/>
       <c r="E42" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2969,7 +3063,7 @@
       <c r="C43" s="7">
         <v>4</v>
       </c>
-      <c r="D43" s="32"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2985,7 +3079,7 @@
       <c r="C44" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="32"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3001,7 +3095,7 @@
       <c r="C45" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="32"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3017,7 +3111,7 @@
       <c r="C46" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D46" s="32"/>
+      <c r="D46" s="37"/>
       <c r="E46" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3033,7 +3127,7 @@
       <c r="C47" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="32"/>
+      <c r="D47" s="37"/>
       <c r="E47" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3050,7 +3144,7 @@
       <c r="C48" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="32"/>
+      <c r="D48" s="37"/>
       <c r="E48" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3067,7 +3161,7 @@
       <c r="C49" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="32"/>
+      <c r="D49" s="37"/>
       <c r="E49" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3084,7 +3178,7 @@
       <c r="C50" s="7">
         <v>16</v>
       </c>
-      <c r="D50" s="32"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3101,7 +3195,7 @@
       <c r="C51" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="32"/>
+      <c r="D51" s="37"/>
       <c r="E51" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3117,7 +3211,7 @@
       <c r="C52" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="32"/>
+      <c r="D52" s="37"/>
       <c r="E52" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3127,13 +3221,13 @@
       <c r="A53" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="28" t="s">
         <v>70</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="32"/>
+      <c r="D53" s="37"/>
       <c r="E53" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3146,10 +3240,10 @@
       <c r="B54" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="32"/>
+      <c r="D54" s="37"/>
       <c r="E54" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3165,7 +3259,7 @@
       <c r="C55" s="7">
         <v>17</v>
       </c>
-      <c r="D55" s="32"/>
+      <c r="D55" s="37"/>
       <c r="E55" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3181,7 +3275,7 @@
       <c r="C56" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="32"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3197,7 +3291,7 @@
       <c r="C57" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="33" t="s">
+      <c r="D57" s="38" t="s">
         <v>292</v>
       </c>
       <c r="E57" s="6" t="str">
@@ -3215,7 +3309,7 @@
       <c r="C58" s="7">
         <v>15</v>
       </c>
-      <c r="D58" s="34"/>
+      <c r="D58" s="39"/>
       <c r="E58" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3231,7 +3325,7 @@
       <c r="C59" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D59" s="34"/>
+      <c r="D59" s="39"/>
       <c r="E59" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3247,7 +3341,7 @@
       <c r="C60" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D60" s="34"/>
+      <c r="D60" s="39"/>
       <c r="E60" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3263,7 +3357,7 @@
       <c r="C61" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D61" s="34"/>
+      <c r="D61" s="39"/>
       <c r="E61" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3279,7 +3373,7 @@
       <c r="C62" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D62" s="34"/>
+      <c r="D62" s="39"/>
       <c r="E62" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3295,7 +3389,7 @@
       <c r="C63" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D63" s="34"/>
+      <c r="D63" s="39"/>
       <c r="E63" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3311,7 +3405,7 @@
       <c r="C64" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="34"/>
+      <c r="D64" s="39"/>
       <c r="E64" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3327,7 +3421,7 @@
       <c r="C65" s="7">
         <v>4</v>
       </c>
-      <c r="D65" s="34"/>
+      <c r="D65" s="39"/>
       <c r="E65" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3343,7 +3437,7 @@
       <c r="C66" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="34"/>
+      <c r="D66" s="39"/>
       <c r="E66" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3359,9 +3453,9 @@
       <c r="C67" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D67" s="34"/>
+      <c r="D67" s="39"/>
       <c r="E67" s="6" t="str">
-        <f t="shared" ref="E67:E128" si="1">IF(AND(B67=C67,B67&lt;&gt;" "),"OK","ERROR")</f>
+        <f t="shared" ref="E67:E130" si="1">IF(AND(B67=C67,B67&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
       </c>
     </row>
@@ -3375,7 +3469,7 @@
       <c r="C68" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D68" s="34"/>
+      <c r="D68" s="39"/>
       <c r="E68" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3391,7 +3485,7 @@
       <c r="C69" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D69" s="34"/>
+      <c r="D69" s="39"/>
       <c r="E69" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3407,7 +3501,7 @@
       <c r="C70" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D70" s="34"/>
+      <c r="D70" s="39"/>
       <c r="E70" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3423,7 +3517,7 @@
       <c r="C71" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="34"/>
+      <c r="D71" s="39"/>
       <c r="E71" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3439,7 +3533,7 @@
       <c r="C72" s="7">
         <v>16</v>
       </c>
-      <c r="D72" s="34"/>
+      <c r="D72" s="39"/>
       <c r="E72" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3455,7 +3549,7 @@
       <c r="C73" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D73" s="34"/>
+      <c r="D73" s="39"/>
       <c r="E73" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3471,7 +3565,7 @@
       <c r="C74" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D74" s="34"/>
+      <c r="D74" s="39"/>
       <c r="E74" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3487,7 +3581,7 @@
       <c r="C75" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D75" s="34"/>
+      <c r="D75" s="39"/>
       <c r="E75" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3503,7 +3597,7 @@
       <c r="C76" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D76" s="34"/>
+      <c r="D76" s="39"/>
       <c r="E76" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3519,7 +3613,7 @@
       <c r="C77" s="7">
         <v>17</v>
       </c>
-      <c r="D77" s="34"/>
+      <c r="D77" s="39"/>
       <c r="E77" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3535,7 +3629,7 @@
       <c r="C78" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D78" s="34"/>
+      <c r="D78" s="39"/>
       <c r="E78" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3551,7 +3645,7 @@
       <c r="C79" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="27" t="s">
+      <c r="D79" s="30" t="s">
         <v>297</v>
       </c>
       <c r="E79" s="6" t="str">
@@ -3569,7 +3663,7 @@
       <c r="C80" s="7">
         <v>7</v>
       </c>
-      <c r="D80" s="27"/>
+      <c r="D80" s="30"/>
       <c r="E80" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3585,7 +3679,7 @@
       <c r="C81" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D81" s="27"/>
+      <c r="D81" s="30"/>
       <c r="E81" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3601,7 +3695,7 @@
       <c r="C82" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D82" s="27"/>
+      <c r="D82" s="30"/>
       <c r="E82" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3617,7 +3711,7 @@
       <c r="C83" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D83" s="27"/>
+      <c r="D83" s="30"/>
       <c r="E83" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3633,7 +3727,7 @@
       <c r="C84" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D84" s="27"/>
+      <c r="D84" s="30"/>
       <c r="E84" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3649,7 +3743,7 @@
       <c r="C85" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D85" s="27"/>
+      <c r="D85" s="30"/>
       <c r="E85" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3665,7 +3759,7 @@
       <c r="C86" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D86" s="27"/>
+      <c r="D86" s="30"/>
       <c r="E86" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3681,7 +3775,7 @@
       <c r="C87" s="7">
         <v>5</v>
       </c>
-      <c r="D87" s="27"/>
+      <c r="D87" s="30"/>
       <c r="E87" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3697,7 +3791,7 @@
       <c r="C88" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D88" s="27"/>
+      <c r="D88" s="30"/>
       <c r="E88" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3713,7 +3807,7 @@
       <c r="C89" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D89" s="27"/>
+      <c r="D89" s="30"/>
       <c r="E89" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3729,7 +3823,7 @@
       <c r="C90" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D90" s="27"/>
+      <c r="D90" s="30"/>
       <c r="E90" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3745,7 +3839,7 @@
       <c r="C91" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D91" s="28" t="s">
+      <c r="D91" s="31" t="s">
         <v>298</v>
       </c>
       <c r="E91" s="6" t="str">
@@ -3763,7 +3857,7 @@
       <c r="C92" s="7">
         <v>7</v>
       </c>
-      <c r="D92" s="29"/>
+      <c r="D92" s="32"/>
       <c r="E92" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3779,7 +3873,7 @@
       <c r="C93" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D93" s="29"/>
+      <c r="D93" s="32"/>
       <c r="E93" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3795,7 +3889,7 @@
       <c r="C94" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D94" s="29"/>
+      <c r="D94" s="32"/>
       <c r="E94" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3811,7 +3905,7 @@
       <c r="C95" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D95" s="29"/>
+      <c r="D95" s="32"/>
       <c r="E95" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3827,7 +3921,7 @@
       <c r="C96" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D96" s="29"/>
+      <c r="D96" s="32"/>
       <c r="E96" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3843,7 +3937,7 @@
       <c r="C97" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D97" s="29"/>
+      <c r="D97" s="32"/>
       <c r="E97" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3859,7 +3953,7 @@
       <c r="C98" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D98" s="29"/>
+      <c r="D98" s="32"/>
       <c r="E98" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3875,7 +3969,7 @@
       <c r="C99" s="7">
         <v>8</v>
       </c>
-      <c r="D99" s="29"/>
+      <c r="D99" s="32"/>
       <c r="E99" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3891,7 +3985,7 @@
       <c r="C100" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D100" s="29"/>
+      <c r="D100" s="32"/>
       <c r="E100" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3907,7 +4001,7 @@
       <c r="C101" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D101" s="29"/>
+      <c r="D101" s="32"/>
       <c r="E101" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3923,7 +4017,7 @@
       <c r="C102" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D102" s="29"/>
+      <c r="D102" s="32"/>
       <c r="E102" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3939,7 +4033,7 @@
       <c r="C103" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D103" s="29"/>
+      <c r="D103" s="32"/>
       <c r="E103" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3955,7 +4049,7 @@
       <c r="C104" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D104" s="29"/>
+      <c r="D104" s="32"/>
       <c r="E104" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3971,7 +4065,7 @@
       <c r="C105" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D105" s="29"/>
+      <c r="D105" s="32"/>
       <c r="E105" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3987,7 +4081,7 @@
       <c r="C106" s="7">
         <v>5</v>
       </c>
-      <c r="D106" s="29"/>
+      <c r="D106" s="32"/>
       <c r="E106" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4003,7 +4097,7 @@
       <c r="C107" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D107" s="29"/>
+      <c r="D107" s="32"/>
       <c r="E107" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4019,7 +4113,7 @@
       <c r="C108" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D108" s="29"/>
+      <c r="D108" s="32"/>
       <c r="E108" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4035,7 +4129,7 @@
       <c r="C109" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D109" s="29"/>
+      <c r="D109" s="33"/>
       <c r="E109" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4051,7 +4145,7 @@
       <c r="C110" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D110" s="30" t="s">
+      <c r="D110" s="34" t="s">
         <v>299</v>
       </c>
       <c r="E110" s="6" t="str">
@@ -4069,7 +4163,7 @@
       <c r="C111" s="7">
         <v>7</v>
       </c>
-      <c r="D111" s="30"/>
+      <c r="D111" s="34"/>
       <c r="E111" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4085,7 +4179,7 @@
       <c r="C112" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D112" s="30"/>
+      <c r="D112" s="34"/>
       <c r="E112" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4101,7 +4195,7 @@
       <c r="C113" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D113" s="30"/>
+      <c r="D113" s="34"/>
       <c r="E113" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4117,7 +4211,7 @@
       <c r="C114" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D114" s="30"/>
+      <c r="D114" s="34"/>
       <c r="E114" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4133,7 +4227,7 @@
       <c r="C115" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D115" s="30"/>
+      <c r="D115" s="34"/>
       <c r="E115" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4149,7 +4243,7 @@
       <c r="C116" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D116" s="30"/>
+      <c r="D116" s="34"/>
       <c r="E116" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4165,7 +4259,7 @@
       <c r="C117" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D117" s="30"/>
+      <c r="D117" s="34"/>
       <c r="E117" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4181,7 +4275,7 @@
       <c r="C118" s="7">
         <v>8</v>
       </c>
-      <c r="D118" s="30"/>
+      <c r="D118" s="34"/>
       <c r="E118" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4197,7 +4291,7 @@
       <c r="C119" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D119" s="30"/>
+      <c r="D119" s="34"/>
       <c r="E119" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4213,7 +4307,7 @@
       <c r="C120" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D120" s="30"/>
+      <c r="D120" s="34"/>
       <c r="E120" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4229,7 +4323,7 @@
       <c r="C121" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D121" s="30"/>
+      <c r="D121" s="34"/>
       <c r="E121" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4245,7 +4339,7 @@
       <c r="C122" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D122" s="30"/>
+      <c r="D122" s="34"/>
       <c r="E122" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4261,7 +4355,7 @@
       <c r="C123" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D123" s="30"/>
+      <c r="D123" s="34"/>
       <c r="E123" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4277,7 +4371,7 @@
       <c r="C124" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D124" s="30"/>
+      <c r="D124" s="34"/>
       <c r="E124" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4293,7 +4387,7 @@
       <c r="C125" s="7">
         <v>5</v>
       </c>
-      <c r="D125" s="30"/>
+      <c r="D125" s="34"/>
       <c r="E125" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4309,7 +4403,7 @@
       <c r="C126" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D126" s="30"/>
+      <c r="D126" s="34"/>
       <c r="E126" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4325,7 +4419,7 @@
       <c r="C127" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D127" s="30"/>
+      <c r="D127" s="34"/>
       <c r="E127" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4341,248 +4435,451 @@
       <c r="C128" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D128" s="30"/>
+      <c r="D128" s="35"/>
       <c r="E128" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D129" s="52" t="s">
+        <v>306</v>
+      </c>
+      <c r="E129" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130" s="8">
+        <v>8</v>
+      </c>
+      <c r="C130" s="7">
+        <v>8</v>
+      </c>
+      <c r="D130" s="53"/>
+      <c r="E130" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D131" s="53"/>
+      <c r="E131" s="6" t="str">
+        <f t="shared" ref="E131:E137" si="2">IF(AND(B131=C131,B131&lt;&gt;" "),"OK","ERROR")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D132" s="53"/>
+      <c r="E132" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133" s="8">
+        <v>8</v>
+      </c>
+      <c r="C133" s="7">
+        <v>8</v>
+      </c>
+      <c r="D133" s="53"/>
+      <c r="E133" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D134" s="53"/>
+      <c r="E134" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D135" s="53"/>
+      <c r="E135" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136" s="8">
+        <v>8</v>
+      </c>
+      <c r="C136" s="7">
+        <v>8</v>
+      </c>
+      <c r="D136" s="53"/>
+      <c r="E136" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D137" s="54"/>
+      <c r="E137" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C138" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C139" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C140" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C141" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C142" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C143" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C144" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C145" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C146" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C147" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C148" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C149" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C150" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C151" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C152" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C153" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C154" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C155" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C156" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C157" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C158" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C159" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C160" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C161" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C162" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C163" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C164" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C165" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C166" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C167" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C168" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C169" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C170" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C171" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>189</v>
       </c>
@@ -5043,7 +5340,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="D129:D137"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D79:D90"/>
@@ -5054,7 +5352,7 @@
     <mergeCell ref="D35:D56"/>
     <mergeCell ref="D57:D78"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:E128">
+  <conditionalFormatting sqref="E2:E137">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$E2="ERROR"</formula>
     </cfRule>
@@ -5093,25 +5391,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="45" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
     </row>
     <row r="2" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>284</v>
       </c>
       <c r="B2" s="16">
@@ -5257,7 +5555,7 @@
       </c>
     </row>
     <row r="3" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="17" t="s">
         <v>32</v>
       </c>
@@ -5331,31 +5629,31 @@
       <c r="AV3" s="17"/>
     </row>
     <row r="4" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="45" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="36" t="s">
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="40" t="s">
         <v>288</v>
       </c>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
     </row>
     <row r="5" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="48" t="s">
         <v>287</v>
       </c>
       <c r="B5" s="16">
@@ -5501,7 +5799,7 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="17" t="s">
         <v>32</v>
       </c>
@@ -5581,41 +5879,41 @@
       <c r="AV6" s="17"/>
     </row>
     <row r="7" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="37" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="40" t="s">
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="44" t="s">
         <v>286</v>
       </c>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="36" t="s">
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="40" t="s">
         <v>288</v>
       </c>
-      <c r="V7" s="36"/>
-      <c r="W7" s="36"/>
-      <c r="X7" s="36"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="40"/>
       <c r="Y7" s="19"/>
     </row>
     <row r="8" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="48" t="s">
         <v>289</v>
       </c>
       <c r="B8" s="16">
@@ -5761,7 +6059,7 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="17" t="s">
         <v>32</v>
       </c>
@@ -5855,41 +6153,41 @@
       <c r="AV9" s="17"/>
     </row>
     <row r="10" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="37" t="s">
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="40" t="s">
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="44" t="s">
         <v>286</v>
       </c>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="41"/>
-      <c r="T10" s="42"/>
-      <c r="U10" s="36" t="s">
+      <c r="Q10" s="45"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="40" t="s">
         <v>288</v>
       </c>
-      <c r="V10" s="36"/>
-      <c r="W10" s="36"/>
-      <c r="X10" s="36"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40"/>
+      <c r="X10" s="40"/>
       <c r="Y10" s="19"/>
     </row>
     <row r="11" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="48" t="s">
         <v>290</v>
       </c>
       <c r="B11" s="16">
@@ -6035,7 +6333,7 @@
       </c>
     </row>
     <row r="12" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="17" t="s">
         <v>32</v>
       </c>
@@ -6159,7 +6457,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6178,27 +6476,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="45" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
       <c r="N1" s="26"/>
       <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:21" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="48" t="s">
         <v>294</v>
       </c>
       <c r="B2" s="16">
@@ -6246,7 +6544,7 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="21" t="s">
         <v>28</v>
       </c>
@@ -6292,34 +6590,34 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="37" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="44" t="s">
         <v>286</v>
       </c>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="42"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="46"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="48" t="s">
         <v>295</v>
       </c>
       <c r="B5" s="16">
@@ -6381,7 +6679,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="21" t="s">
         <v>28</v>
       </c>
@@ -6441,34 +6739,34 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="37" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
-      <c r="P7" s="40" t="s">
+      <c r="P7" s="44" t="s">
         <v>286</v>
       </c>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="42"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="46"/>
     </row>
     <row r="8" spans="1:21" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="48" t="s">
         <v>296</v>
       </c>
       <c r="B8" s="16">
@@ -6530,7 +6828,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="48"/>
       <c r="B9" s="21" t="s">
         <v>28</v>
       </c>
@@ -6611,4 +6909,187 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="14" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+    </row>
+    <row r="2" spans="1:12" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16">
+        <v>2</v>
+      </c>
+      <c r="D2" s="16">
+        <v>3</v>
+      </c>
+      <c r="E2" s="16">
+        <v>4</v>
+      </c>
+      <c r="F2" s="16">
+        <v>5</v>
+      </c>
+      <c r="G2" s="16">
+        <v>6</v>
+      </c>
+      <c r="H2" s="16">
+        <v>7</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="48"/>
+      <c r="B3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="23">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="23">
+        <v>10</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+    </row>
+    <row r="6" spans="1:12" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="B6" s="16">
+        <v>128</v>
+      </c>
+      <c r="C6" s="16">
+        <v>129</v>
+      </c>
+      <c r="D6" s="16">
+        <v>130</v>
+      </c>
+      <c r="E6" s="16">
+        <v>131</v>
+      </c>
+      <c r="F6" s="16">
+        <v>132</v>
+      </c>
+      <c r="G6" s="16">
+        <v>133</v>
+      </c>
+      <c r="H6" s="16">
+        <v>134</v>
+      </c>
+      <c r="I6" s="16">
+        <v>135</v>
+      </c>
+      <c r="J6" s="16">
+        <v>136</v>
+      </c>
+      <c r="K6" s="16">
+        <v>137</v>
+      </c>
+      <c r="L6" s="16">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="48"/>
+      <c r="B7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="23">
+        <v>8</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="23">
+        <v>8</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="23">
+        <v>8</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A6:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FIX en lectura de tokens
Faltaba insertar token STRING y REAL a la GCI
</commit_message>
<xml_diff>
--- a/Segunda_entrega/CHECK.xlsx
+++ b/Segunda_entrega/CHECK.xlsx
@@ -15,7 +15,7 @@
     <sheet name="TEST COMPLETO" sheetId="2" r:id="rId1"/>
     <sheet name="TEST-IF" sheetId="3" r:id="rId2"/>
     <sheet name="TEST-WHILE" sheetId="4" r:id="rId3"/>
-    <sheet name="TEST-ASIGMUL" sheetId="5" r:id="rId4"/>
+    <sheet name="TEST-ASIGMUL-BETWEEN" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -668,7 +668,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="308">
   <si>
     <t>CELDA 1</t>
   </si>
@@ -1574,9 +1574,6 @@
   </si>
   <si>
     <t>*</t>
-  </si>
-  <si>
-    <t>###</t>
   </si>
   <si>
     <t>i:=1 
@@ -1590,6 +1587,12 @@
   </si>
   <si>
     <t>ASIGNACION MULTIPLE</t>
+  </si>
+  <si>
+    <t>BETWEEN (a,[2;a*(b+4)])</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1942,6 +1945,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1975,6 +1993,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1994,30 +2021,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2349,10 +2352,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2384,13 +2390,13 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="34" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="6" t="str">
@@ -2409,13 +2415,13 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="29"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="6" t="str">
         <f t="shared" ref="E3:E66" si="0">IF(AND(B3=C3,B3&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -2425,13 +2431,13 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2441,13 +2447,13 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="34" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="6" t="str">
@@ -2459,13 +2465,13 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="9">
         <v>10</v>
       </c>
       <c r="C6" s="7">
         <v>10</v>
       </c>
-      <c r="D6" s="29"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2475,13 +2481,13 @@
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2497,7 +2503,7 @@
       <c r="C8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="41" t="s">
         <v>281</v>
       </c>
       <c r="E8" s="6" t="str">
@@ -2515,7 +2521,7 @@
       <c r="C9" s="7">
         <v>15</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2531,7 +2537,7 @@
       <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="36"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2547,7 +2553,7 @@
       <c r="C11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="36"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2563,7 +2569,7 @@
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="36"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2579,7 +2585,7 @@
       <c r="C13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="36"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2595,7 +2601,7 @@
       <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2611,7 +2617,7 @@
       <c r="C15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="41"/>
       <c r="E15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2627,7 +2633,7 @@
       <c r="C16" s="7">
         <v>16</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2643,7 +2649,7 @@
       <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="36"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2659,7 +2665,7 @@
       <c r="C18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="36"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2675,7 +2681,7 @@
       <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="36"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2691,7 +2697,7 @@
       <c r="C20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="36" t="s">
         <v>282</v>
       </c>
       <c r="E20" s="6" t="str">
@@ -2709,7 +2715,7 @@
       <c r="C21" s="7">
         <v>15</v>
       </c>
-      <c r="D21" s="32"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2725,7 +2731,7 @@
       <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="32"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2741,7 +2747,7 @@
       <c r="C23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2757,7 +2763,7 @@
       <c r="C24" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2773,7 +2779,7 @@
       <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2789,7 +2795,7 @@
       <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="32"/>
+      <c r="D26" s="37"/>
       <c r="E26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2805,7 +2811,7 @@
       <c r="C27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2821,7 +2827,7 @@
       <c r="C28" s="7">
         <v>16</v>
       </c>
-      <c r="D28" s="32"/>
+      <c r="D28" s="37"/>
       <c r="E28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2837,7 +2843,7 @@
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="32"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2853,7 +2859,7 @@
       <c r="C30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="32"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2869,7 +2875,7 @@
       <c r="C31" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="32"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2885,7 +2891,7 @@
       <c r="C32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2901,7 +2907,7 @@
       <c r="C33" s="7">
         <v>17</v>
       </c>
-      <c r="D33" s="32"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2917,7 +2923,7 @@
       <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="32"/>
+      <c r="D34" s="37"/>
       <c r="E34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2933,7 +2939,7 @@
       <c r="C35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="36" t="s">
+      <c r="D35" s="41" t="s">
         <v>291</v>
       </c>
       <c r="E35" s="6" t="str">
@@ -2951,7 +2957,7 @@
       <c r="C36" s="7">
         <v>15</v>
       </c>
-      <c r="D36" s="37"/>
+      <c r="D36" s="42"/>
       <c r="E36" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2967,7 +2973,7 @@
       <c r="C37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="37"/>
+      <c r="D37" s="42"/>
       <c r="E37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2983,7 +2989,7 @@
       <c r="C38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="37"/>
+      <c r="D38" s="42"/>
       <c r="E38" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2999,7 +3005,7 @@
       <c r="C39" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="37"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3015,7 +3021,7 @@
       <c r="C40" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="37"/>
+      <c r="D40" s="42"/>
       <c r="E40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3031,7 +3037,7 @@
       <c r="C41" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D41" s="37"/>
+      <c r="D41" s="42"/>
       <c r="E41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3047,7 +3053,7 @@
       <c r="C42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="37"/>
+      <c r="D42" s="42"/>
       <c r="E42" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3063,7 +3069,7 @@
       <c r="C43" s="7">
         <v>4</v>
       </c>
-      <c r="D43" s="37"/>
+      <c r="D43" s="42"/>
       <c r="E43" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3079,7 +3085,7 @@
       <c r="C44" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="37"/>
+      <c r="D44" s="42"/>
       <c r="E44" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3095,7 +3101,7 @@
       <c r="C45" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="37"/>
+      <c r="D45" s="42"/>
       <c r="E45" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3111,7 +3117,7 @@
       <c r="C46" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D46" s="37"/>
+      <c r="D46" s="42"/>
       <c r="E46" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3127,7 +3133,7 @@
       <c r="C47" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="37"/>
+      <c r="D47" s="42"/>
       <c r="E47" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3144,7 +3150,7 @@
       <c r="C48" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="37"/>
+      <c r="D48" s="42"/>
       <c r="E48" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3161,7 +3167,7 @@
       <c r="C49" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="37"/>
+      <c r="D49" s="42"/>
       <c r="E49" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3178,7 +3184,7 @@
       <c r="C50" s="7">
         <v>16</v>
       </c>
-      <c r="D50" s="37"/>
+      <c r="D50" s="42"/>
       <c r="E50" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3195,7 +3201,7 @@
       <c r="C51" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="37"/>
+      <c r="D51" s="42"/>
       <c r="E51" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3211,7 +3217,7 @@
       <c r="C52" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="37"/>
+      <c r="D52" s="42"/>
       <c r="E52" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3227,7 +3233,7 @@
       <c r="C53" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D53" s="37"/>
+      <c r="D53" s="42"/>
       <c r="E53" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3243,7 +3249,7 @@
       <c r="C54" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="37"/>
+      <c r="D54" s="42"/>
       <c r="E54" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3259,7 +3265,7 @@
       <c r="C55" s="7">
         <v>17</v>
       </c>
-      <c r="D55" s="37"/>
+      <c r="D55" s="42"/>
       <c r="E55" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3275,7 +3281,7 @@
       <c r="C56" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="37"/>
+      <c r="D56" s="42"/>
       <c r="E56" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3291,7 +3297,7 @@
       <c r="C57" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="38" t="s">
+      <c r="D57" s="43" t="s">
         <v>292</v>
       </c>
       <c r="E57" s="6" t="str">
@@ -3309,7 +3315,7 @@
       <c r="C58" s="7">
         <v>15</v>
       </c>
-      <c r="D58" s="39"/>
+      <c r="D58" s="44"/>
       <c r="E58" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3325,7 +3331,7 @@
       <c r="C59" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D59" s="39"/>
+      <c r="D59" s="44"/>
       <c r="E59" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3341,7 +3347,7 @@
       <c r="C60" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D60" s="39"/>
+      <c r="D60" s="44"/>
       <c r="E60" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3357,7 +3363,7 @@
       <c r="C61" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D61" s="39"/>
+      <c r="D61" s="44"/>
       <c r="E61" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3373,7 +3379,7 @@
       <c r="C62" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D62" s="39"/>
+      <c r="D62" s="44"/>
       <c r="E62" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3389,7 +3395,7 @@
       <c r="C63" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D63" s="39"/>
+      <c r="D63" s="44"/>
       <c r="E63" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3405,7 +3411,7 @@
       <c r="C64" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="39"/>
+      <c r="D64" s="44"/>
       <c r="E64" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3421,7 +3427,7 @@
       <c r="C65" s="7">
         <v>4</v>
       </c>
-      <c r="D65" s="39"/>
+      <c r="D65" s="44"/>
       <c r="E65" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3437,7 +3443,7 @@
       <c r="C66" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="39"/>
+      <c r="D66" s="44"/>
       <c r="E66" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3453,7 +3459,7 @@
       <c r="C67" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D67" s="39"/>
+      <c r="D67" s="44"/>
       <c r="E67" s="6" t="str">
         <f t="shared" ref="E67:E130" si="1">IF(AND(B67=C67,B67&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -3469,7 +3475,7 @@
       <c r="C68" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D68" s="39"/>
+      <c r="D68" s="44"/>
       <c r="E68" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3485,7 +3491,7 @@
       <c r="C69" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D69" s="39"/>
+      <c r="D69" s="44"/>
       <c r="E69" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3501,7 +3507,7 @@
       <c r="C70" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D70" s="39"/>
+      <c r="D70" s="44"/>
       <c r="E70" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3517,7 +3523,7 @@
       <c r="C71" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="39"/>
+      <c r="D71" s="44"/>
       <c r="E71" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3533,7 +3539,7 @@
       <c r="C72" s="7">
         <v>16</v>
       </c>
-      <c r="D72" s="39"/>
+      <c r="D72" s="44"/>
       <c r="E72" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3549,7 +3555,7 @@
       <c r="C73" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D73" s="39"/>
+      <c r="D73" s="44"/>
       <c r="E73" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3565,7 +3571,7 @@
       <c r="C74" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D74" s="39"/>
+      <c r="D74" s="44"/>
       <c r="E74" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3581,7 +3587,7 @@
       <c r="C75" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D75" s="39"/>
+      <c r="D75" s="44"/>
       <c r="E75" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3597,7 +3603,7 @@
       <c r="C76" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D76" s="39"/>
+      <c r="D76" s="44"/>
       <c r="E76" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3613,7 +3619,7 @@
       <c r="C77" s="7">
         <v>17</v>
       </c>
-      <c r="D77" s="39"/>
+      <c r="D77" s="44"/>
       <c r="E77" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3629,7 +3635,7 @@
       <c r="C78" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D78" s="39"/>
+      <c r="D78" s="44"/>
       <c r="E78" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3645,7 +3651,7 @@
       <c r="C79" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="30" t="s">
+      <c r="D79" s="35" t="s">
         <v>297</v>
       </c>
       <c r="E79" s="6" t="str">
@@ -3663,7 +3669,7 @@
       <c r="C80" s="7">
         <v>7</v>
       </c>
-      <c r="D80" s="30"/>
+      <c r="D80" s="35"/>
       <c r="E80" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3679,7 +3685,7 @@
       <c r="C81" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D81" s="30"/>
+      <c r="D81" s="35"/>
       <c r="E81" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3695,7 +3701,7 @@
       <c r="C82" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D82" s="30"/>
+      <c r="D82" s="35"/>
       <c r="E82" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3711,7 +3717,7 @@
       <c r="C83" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D83" s="30"/>
+      <c r="D83" s="35"/>
       <c r="E83" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3727,7 +3733,7 @@
       <c r="C84" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D84" s="30"/>
+      <c r="D84" s="35"/>
       <c r="E84" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3743,7 +3749,7 @@
       <c r="C85" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D85" s="30"/>
+      <c r="D85" s="35"/>
       <c r="E85" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3759,7 +3765,7 @@
       <c r="C86" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D86" s="30"/>
+      <c r="D86" s="35"/>
       <c r="E86" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3775,7 +3781,7 @@
       <c r="C87" s="7">
         <v>5</v>
       </c>
-      <c r="D87" s="30"/>
+      <c r="D87" s="35"/>
       <c r="E87" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3791,7 +3797,7 @@
       <c r="C88" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D88" s="30"/>
+      <c r="D88" s="35"/>
       <c r="E88" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3807,7 +3813,7 @@
       <c r="C89" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D89" s="30"/>
+      <c r="D89" s="35"/>
       <c r="E89" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3823,7 +3829,7 @@
       <c r="C90" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D90" s="30"/>
+      <c r="D90" s="35"/>
       <c r="E90" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3839,7 +3845,7 @@
       <c r="C91" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D91" s="31" t="s">
+      <c r="D91" s="36" t="s">
         <v>298</v>
       </c>
       <c r="E91" s="6" t="str">
@@ -3857,7 +3863,7 @@
       <c r="C92" s="7">
         <v>7</v>
       </c>
-      <c r="D92" s="32"/>
+      <c r="D92" s="37"/>
       <c r="E92" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3873,7 +3879,7 @@
       <c r="C93" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D93" s="32"/>
+      <c r="D93" s="37"/>
       <c r="E93" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3889,7 +3895,7 @@
       <c r="C94" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D94" s="32"/>
+      <c r="D94" s="37"/>
       <c r="E94" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3905,7 +3911,7 @@
       <c r="C95" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D95" s="32"/>
+      <c r="D95" s="37"/>
       <c r="E95" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3921,7 +3927,7 @@
       <c r="C96" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D96" s="32"/>
+      <c r="D96" s="37"/>
       <c r="E96" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3937,7 +3943,7 @@
       <c r="C97" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D97" s="32"/>
+      <c r="D97" s="37"/>
       <c r="E97" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3953,7 +3959,7 @@
       <c r="C98" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D98" s="32"/>
+      <c r="D98" s="37"/>
       <c r="E98" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3969,7 +3975,7 @@
       <c r="C99" s="7">
         <v>8</v>
       </c>
-      <c r="D99" s="32"/>
+      <c r="D99" s="37"/>
       <c r="E99" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3985,7 +3991,7 @@
       <c r="C100" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D100" s="32"/>
+      <c r="D100" s="37"/>
       <c r="E100" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4001,7 +4007,7 @@
       <c r="C101" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D101" s="32"/>
+      <c r="D101" s="37"/>
       <c r="E101" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4017,7 +4023,7 @@
       <c r="C102" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D102" s="32"/>
+      <c r="D102" s="37"/>
       <c r="E102" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4033,7 +4039,7 @@
       <c r="C103" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D103" s="32"/>
+      <c r="D103" s="37"/>
       <c r="E103" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4049,7 +4055,7 @@
       <c r="C104" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D104" s="32"/>
+      <c r="D104" s="37"/>
       <c r="E104" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4065,7 +4071,7 @@
       <c r="C105" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D105" s="32"/>
+      <c r="D105" s="37"/>
       <c r="E105" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4081,7 +4087,7 @@
       <c r="C106" s="7">
         <v>5</v>
       </c>
-      <c r="D106" s="32"/>
+      <c r="D106" s="37"/>
       <c r="E106" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4097,7 +4103,7 @@
       <c r="C107" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D107" s="32"/>
+      <c r="D107" s="37"/>
       <c r="E107" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4113,7 +4119,7 @@
       <c r="C108" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D108" s="32"/>
+      <c r="D108" s="37"/>
       <c r="E108" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4129,7 +4135,7 @@
       <c r="C109" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D109" s="33"/>
+      <c r="D109" s="38"/>
       <c r="E109" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4145,7 +4151,7 @@
       <c r="C110" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D110" s="34" t="s">
+      <c r="D110" s="39" t="s">
         <v>299</v>
       </c>
       <c r="E110" s="6" t="str">
@@ -4163,7 +4169,7 @@
       <c r="C111" s="7">
         <v>7</v>
       </c>
-      <c r="D111" s="34"/>
+      <c r="D111" s="39"/>
       <c r="E111" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4179,7 +4185,7 @@
       <c r="C112" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D112" s="34"/>
+      <c r="D112" s="39"/>
       <c r="E112" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4195,7 +4201,7 @@
       <c r="C113" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D113" s="34"/>
+      <c r="D113" s="39"/>
       <c r="E113" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4211,7 +4217,7 @@
       <c r="C114" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D114" s="34"/>
+      <c r="D114" s="39"/>
       <c r="E114" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4227,7 +4233,7 @@
       <c r="C115" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D115" s="34"/>
+      <c r="D115" s="39"/>
       <c r="E115" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4243,7 +4249,7 @@
       <c r="C116" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D116" s="34"/>
+      <c r="D116" s="39"/>
       <c r="E116" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4259,7 +4265,7 @@
       <c r="C117" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D117" s="34"/>
+      <c r="D117" s="39"/>
       <c r="E117" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4275,7 +4281,7 @@
       <c r="C118" s="7">
         <v>8</v>
       </c>
-      <c r="D118" s="34"/>
+      <c r="D118" s="39"/>
       <c r="E118" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4291,7 +4297,7 @@
       <c r="C119" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D119" s="34"/>
+      <c r="D119" s="39"/>
       <c r="E119" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4307,7 +4313,7 @@
       <c r="C120" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D120" s="34"/>
+      <c r="D120" s="39"/>
       <c r="E120" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4323,7 +4329,7 @@
       <c r="C121" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D121" s="34"/>
+      <c r="D121" s="39"/>
       <c r="E121" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4339,7 +4345,7 @@
       <c r="C122" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D122" s="34"/>
+      <c r="D122" s="39"/>
       <c r="E122" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4355,7 +4361,7 @@
       <c r="C123" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D123" s="34"/>
+      <c r="D123" s="39"/>
       <c r="E123" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4371,7 +4377,7 @@
       <c r="C124" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D124" s="34"/>
+      <c r="D124" s="39"/>
       <c r="E124" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4387,7 +4393,7 @@
       <c r="C125" s="7">
         <v>5</v>
       </c>
-      <c r="D125" s="34"/>
+      <c r="D125" s="39"/>
       <c r="E125" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4403,7 +4409,7 @@
       <c r="C126" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D126" s="34"/>
+      <c r="D126" s="39"/>
       <c r="E126" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4419,7 +4425,7 @@
       <c r="C127" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D127" s="34"/>
+      <c r="D127" s="39"/>
       <c r="E127" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4435,7 +4441,7 @@
       <c r="C128" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D128" s="35"/>
+      <c r="D128" s="40"/>
       <c r="E128" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4451,8 +4457,8 @@
       <c r="C129" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D129" s="52" t="s">
-        <v>306</v>
+      <c r="D129" s="31" t="s">
+        <v>305</v>
       </c>
       <c r="E129" s="6" t="str">
         <f t="shared" si="1"/>
@@ -4469,7 +4475,7 @@
       <c r="C130" s="7">
         <v>8</v>
       </c>
-      <c r="D130" s="53"/>
+      <c r="D130" s="32"/>
       <c r="E130" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4485,7 +4491,7 @@
       <c r="C131" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D131" s="53"/>
+      <c r="D131" s="32"/>
       <c r="E131" s="6" t="str">
         <f t="shared" ref="E131:E137" si="2">IF(AND(B131=C131,B131&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -4501,7 +4507,7 @@
       <c r="C132" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D132" s="53"/>
+      <c r="D132" s="32"/>
       <c r="E132" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4517,7 +4523,7 @@
       <c r="C133" s="7">
         <v>8</v>
       </c>
-      <c r="D133" s="53"/>
+      <c r="D133" s="32"/>
       <c r="E133" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4533,7 +4539,7 @@
       <c r="C134" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D134" s="53"/>
+      <c r="D134" s="32"/>
       <c r="E134" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4549,7 +4555,7 @@
       <c r="C135" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D135" s="53"/>
+      <c r="D135" s="32"/>
       <c r="E135" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4565,7 +4571,7 @@
       <c r="C136" s="7">
         <v>8</v>
       </c>
-      <c r="D136" s="53"/>
+      <c r="D136" s="32"/>
       <c r="E136" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4581,7 +4587,7 @@
       <c r="C137" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D137" s="54"/>
+      <c r="D137" s="33"/>
       <c r="E137" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4591,32 +4597,32 @@
       <c r="A138" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C138" s="7">
-        <v>8</v>
+      <c r="C138" s="7" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C139" s="7" t="s">
-        <v>33</v>
+      <c r="C139" s="7">
+        <v>8</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C140" s="7">
-        <v>2</v>
+      <c r="C140" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C141" s="7" t="s">
-        <v>28</v>
+      <c r="C141" s="7">
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4624,7 +4630,7 @@
         <v>155</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4632,7 +4638,7 @@
         <v>156</v>
       </c>
       <c r="C143" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4640,7 +4646,7 @@
         <v>157</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -4648,15 +4654,15 @@
         <v>158</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>301</v>
+        <v>34</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C146" s="7" t="s">
-        <v>33</v>
+      <c r="C146" s="7">
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -4664,7 +4670,7 @@
         <v>160</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -4672,7 +4678,7 @@
         <v>161</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -5391,25 +5397,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="49" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="47" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
     </row>
     <row r="2" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>284</v>
       </c>
       <c r="B2" s="16">
@@ -5555,7 +5561,7 @@
       </c>
     </row>
     <row r="3" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="17" t="s">
         <v>32</v>
       </c>
@@ -5629,31 +5635,31 @@
       <c r="AV3" s="17"/>
     </row>
     <row r="4" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="49" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="47" t="s">
         <v>286</v>
       </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="40" t="s">
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48" t="s">
         <v>288</v>
       </c>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
     </row>
     <row r="5" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="45" t="s">
         <v>287</v>
       </c>
       <c r="B5" s="16">
@@ -5799,7 +5805,7 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="17" t="s">
         <v>32</v>
       </c>
@@ -5879,41 +5885,41 @@
       <c r="AV6" s="17"/>
     </row>
     <row r="7" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="41" t="s">
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="44" t="s">
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="52" t="s">
         <v>286</v>
       </c>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="46"/>
-      <c r="U7" s="40" t="s">
+      <c r="Q7" s="53"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="54"/>
+      <c r="U7" s="48" t="s">
         <v>288</v>
       </c>
-      <c r="V7" s="40"/>
-      <c r="W7" s="40"/>
-      <c r="X7" s="40"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
       <c r="Y7" s="19"/>
     </row>
     <row r="8" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="45" t="s">
         <v>289</v>
       </c>
       <c r="B8" s="16">
@@ -6059,7 +6065,7 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="17" t="s">
         <v>32</v>
       </c>
@@ -6153,41 +6159,41 @@
       <c r="AV9" s="17"/>
     </row>
     <row r="10" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="41" t="s">
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="44" t="s">
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="52" t="s">
         <v>286</v>
       </c>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="46"/>
-      <c r="U10" s="40" t="s">
+      <c r="Q10" s="53"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="53"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="48" t="s">
         <v>288</v>
       </c>
-      <c r="V10" s="40"/>
-      <c r="W10" s="40"/>
-      <c r="X10" s="40"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
       <c r="Y10" s="19"/>
     </row>
     <row r="11" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="45" t="s">
         <v>290</v>
       </c>
       <c r="B11" s="16">
@@ -6333,7 +6339,7 @@
       </c>
     </row>
     <row r="12" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="17" t="s">
         <v>32</v>
       </c>
@@ -6428,11 +6434,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="I10:O10"/>
+    <mergeCell ref="P10:T10"/>
+    <mergeCell ref="U10:X10"/>
+    <mergeCell ref="B10:H10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="N4:Q4"/>
@@ -6440,11 +6446,11 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="P7:T7"/>
-    <mergeCell ref="U7:X7"/>
-    <mergeCell ref="I10:O10"/>
-    <mergeCell ref="P10:T10"/>
-    <mergeCell ref="U10:X10"/>
-    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="I4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6476,27 +6482,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="49" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="47" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
       <c r="N1" s="26"/>
       <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:21" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>294</v>
       </c>
       <c r="B2" s="16">
@@ -6544,7 +6550,7 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="21" t="s">
         <v>28</v>
       </c>
@@ -6590,34 +6596,34 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="41" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
-      <c r="P4" s="44" t="s">
+      <c r="P4" s="52" t="s">
         <v>286</v>
       </c>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="46"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="54"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="45" t="s">
         <v>295</v>
       </c>
       <c r="B5" s="16">
@@ -6679,7 +6685,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="21" t="s">
         <v>28</v>
       </c>
@@ -6739,34 +6745,34 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="41" t="s">
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
-      <c r="P7" s="44" t="s">
+      <c r="P7" s="52" t="s">
         <v>286</v>
       </c>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="46"/>
+      <c r="Q7" s="53"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="54"/>
     </row>
     <row r="8" spans="1:21" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="45" t="s">
         <v>296</v>
       </c>
       <c r="B8" s="16">
@@ -6828,7 +6834,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="21" t="s">
         <v>28</v>
       </c>
@@ -6895,17 +6901,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="P7:T7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="I4:M4"/>
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="P7:T7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6913,10 +6919,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A12" sqref="A12:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6925,16 +6931,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="14" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:12" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>303</v>
+      <c r="A2" s="45" t="s">
+        <v>302</v>
       </c>
       <c r="B2" s="16">
         <v>1</v>
@@ -6963,7 +6969,7 @@
       <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:12" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="21" t="s">
         <v>32</v>
       </c>
@@ -6990,28 +6996,28 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
+        <v>303</v>
+      </c>
+      <c r="H4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+    </row>
+    <row r="6" spans="1:12" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
         <v>304</v>
-      </c>
-      <c r="H4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-    </row>
-    <row r="6" spans="1:12" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
-        <v>305</v>
       </c>
       <c r="B6" s="16">
         <v>128</v>
@@ -7048,7 +7054,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="21" t="s">
         <v>28</v>
       </c>
@@ -7081,14 +7087,81 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
-        <v>304</v>
-      </c>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="45" t="s">
+        <v>306</v>
+      </c>
+      <c r="B12" s="16">
+        <v>128</v>
+      </c>
+      <c r="C12" s="16">
+        <v>129</v>
+      </c>
+      <c r="D12" s="16">
+        <v>130</v>
+      </c>
+      <c r="E12" s="16">
+        <v>131</v>
+      </c>
+      <c r="F12" s="16">
+        <v>132</v>
+      </c>
+      <c r="G12" s="16">
+        <v>133</v>
+      </c>
+      <c r="H12" s="16">
+        <v>134</v>
+      </c>
+      <c r="I12" s="16">
+        <v>135</v>
+      </c>
+      <c r="J12" s="16">
+        <v>136</v>
+      </c>
+      <c r="K12" s="16">
+        <v>137</v>
+      </c>
+      <c r="L12" s="16">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixes y algunos comentarios en codigo
Falta el BETWEEN entre otras cosas.
</commit_message>
<xml_diff>
--- a/Segunda_entrega/CHECK.xlsx
+++ b/Segunda_entrega/CHECK.xlsx
@@ -1993,15 +1993,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2021,6 +2012,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2357,8 +2357,8 @@
   </sheetPr>
   <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5397,25 +5397,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="52" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="54" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
     </row>
     <row r="2" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="53" t="s">
         <v>284</v>
       </c>
       <c r="B2" s="16">
@@ -5561,7 +5561,7 @@
       </c>
     </row>
     <row r="3" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="17" t="s">
         <v>32</v>
       </c>
@@ -5635,31 +5635,31 @@
       <c r="AV3" s="17"/>
     </row>
     <row r="4" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="52" t="s">
         <v>285</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="54" t="s">
         <v>286</v>
       </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="48" t="s">
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="45" t="s">
         <v>288</v>
       </c>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
     </row>
     <row r="5" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="53" t="s">
         <v>287</v>
       </c>
       <c r="B5" s="16">
@@ -5805,7 +5805,7 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="17" t="s">
         <v>32</v>
       </c>
@@ -5885,41 +5885,41 @@
       <c r="AV6" s="17"/>
     </row>
     <row r="7" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="52" t="s">
         <v>285</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="49" t="s">
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="52" t="s">
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="54"/>
-      <c r="U7" s="48" t="s">
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="51"/>
+      <c r="U7" s="45" t="s">
         <v>288</v>
       </c>
-      <c r="V7" s="48"/>
-      <c r="W7" s="48"/>
-      <c r="X7" s="48"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
       <c r="Y7" s="19"/>
     </row>
     <row r="8" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="53" t="s">
         <v>289</v>
       </c>
       <c r="B8" s="16">
@@ -6065,7 +6065,7 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="17" t="s">
         <v>32</v>
       </c>
@@ -6159,41 +6159,41 @@
       <c r="AV9" s="17"/>
     </row>
     <row r="10" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="52" t="s">
         <v>285</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="49" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="52" t="s">
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="53"/>
-      <c r="T10" s="54"/>
-      <c r="U10" s="48" t="s">
+      <c r="Q10" s="50"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="45" t="s">
         <v>288</v>
       </c>
-      <c r="V10" s="48"/>
-      <c r="W10" s="48"/>
-      <c r="X10" s="48"/>
+      <c r="V10" s="45"/>
+      <c r="W10" s="45"/>
+      <c r="X10" s="45"/>
       <c r="Y10" s="19"/>
     </row>
     <row r="11" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="53" t="s">
         <v>290</v>
       </c>
       <c r="B11" s="16">
@@ -6339,7 +6339,7 @@
       </c>
     </row>
     <row r="12" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="17" t="s">
         <v>32</v>
       </c>
@@ -6434,11 +6434,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="U7:X7"/>
-    <mergeCell ref="I10:O10"/>
-    <mergeCell ref="P10:T10"/>
-    <mergeCell ref="U10:X10"/>
-    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="I4:M4"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="N4:Q4"/>
@@ -6446,11 +6446,11 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="P7:T7"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="I10:O10"/>
+    <mergeCell ref="P10:T10"/>
+    <mergeCell ref="U10:X10"/>
+    <mergeCell ref="B10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6482,27 +6482,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="52" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="54" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
       <c r="N1" s="26"/>
       <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:21" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="53" t="s">
         <v>294</v>
       </c>
       <c r="B2" s="16">
@@ -6550,7 +6550,7 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="21" t="s">
         <v>28</v>
       </c>
@@ -6596,34 +6596,34 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="52" t="s">
         <v>285</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="49" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="54"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="51"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="53" t="s">
         <v>295</v>
       </c>
       <c r="B5" s="16">
@@ -6685,7 +6685,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="21" t="s">
         <v>28</v>
       </c>
@@ -6745,34 +6745,34 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="52" t="s">
         <v>285</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="49" t="s">
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
-      <c r="P7" s="52" t="s">
+      <c r="P7" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="54"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="51"/>
     </row>
     <row r="8" spans="1:21" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="53" t="s">
         <v>296</v>
       </c>
       <c r="B8" s="16">
@@ -6834,7 +6834,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="21" t="s">
         <v>28</v>
       </c>
@@ -6901,17 +6901,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="P7:T7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="I4:M4"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="P7:T7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6931,15 +6931,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="14" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:12" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="53" t="s">
         <v>302</v>
       </c>
       <c r="B2" s="16">
@@ -6969,7 +6969,7 @@
       <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:12" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="21" t="s">
         <v>32</v>
       </c>
@@ -7016,7 +7016,7 @@
       <c r="L5" s="30"/>
     </row>
     <row r="6" spans="1:12" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="53" t="s">
         <v>304</v>
       </c>
       <c r="B6" s="16">
@@ -7054,7 +7054,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="21" t="s">
         <v>28</v>
       </c>
@@ -7105,7 +7105,7 @@
       <c r="L11" s="30"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="53" t="s">
         <v>306</v>
       </c>
       <c r="B12" s="16">
@@ -7143,7 +7143,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>

</xml_diff>